<commit_message>
new start (version 0.0.10) after CRAN submission of version 0.0.9
</commit_message>
<xml_diff>
--- a/man/tables/ae_detail_EXAMPLE_STUDY_Cohort_A_30OCT2020.xlsx
+++ b/man/tables/ae_detail_EXAMPLE_STUDY_Cohort_A_30OCT2020.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="83">
   <si>
     <t xml:space="preserve">Category</t>
   </si>
@@ -23,13 +23,13 @@
     <t xml:space="preserve"># of subjects that have experienced the AE</t>
   </si>
   <si>
-    <t xml:space="preserve">the % of subjects that this comprises of the total accrual (N=2)</t>
+    <t xml:space="preserve">the % of subjects that this comprises of the total accrual (N=3)</t>
   </si>
   <si>
     <t xml:space="preserve"># of subjects that experienced the event at a grade 3 to 5</t>
   </si>
   <si>
-    <t xml:space="preserve">% of the subjects that this comprises of the total accrual (N=2)</t>
+    <t xml:space="preserve">% of the subjects that this comprises of the total accrual (N=3)</t>
   </si>
   <si>
     <t xml:space="preserve">BLOOD AND LYMPHATIC SYSTEM DISORDERS</t>
@@ -38,22 +38,19 @@
     <t xml:space="preserve">ANEMIA</t>
   </si>
   <si>
-    <t xml:space="preserve"> 50.00</t>
+    <t xml:space="preserve">33.33</t>
   </si>
   <si>
     <t xml:space="preserve">FEBRILE NEUTROPENIA</t>
   </si>
   <si>
-    <t xml:space="preserve">100.00</t>
+    <t xml:space="preserve">66.67</t>
   </si>
   <si>
     <t xml:space="preserve">ENDOCRINE DISORDERS</t>
   </si>
   <si>
     <t xml:space="preserve">THYROID NODULE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50.00</t>
   </si>
   <si>
     <t xml:space="preserve">0</t>
@@ -794,22 +791,22 @@
   <sheetData>
     <row r="1" ht="50" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" ht="82" customHeight="1">
@@ -883,42 +880,42 @@
         <v>1</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="C13" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E13" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C14" s="3" t="n">
         <v>1</v>
       </c>
@@ -929,15 +926,15 @@
         <v>0</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="3" t="n">
         <v>1</v>
@@ -949,15 +946,15 @@
         <v>0</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>2</v>
@@ -969,15 +966,15 @@
         <v>0</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C17" s="3" t="n">
         <v>1</v>
@@ -989,316 +986,316 @@
         <v>0</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="C18" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E18" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E19" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E20" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="C21" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E21" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E22" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E23" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E24" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>32</v>
-      </c>
       <c r="C25" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E25" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C26" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E26" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C27" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E27" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C28" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E28" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E29" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E30" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E31" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E32" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>42</v>
-      </c>
       <c r="C33" s="3" t="n">
         <v>1</v>
       </c>
@@ -1309,15 +1306,15 @@
         <v>1</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C34" s="3" t="n">
         <v>1</v>
@@ -1329,15 +1326,15 @@
         <v>0</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C35" s="3" t="n">
         <v>1</v>
@@ -1349,15 +1346,15 @@
         <v>0</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C36" s="3" t="n">
         <v>2</v>
@@ -1369,15 +1366,15 @@
         <v>0</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C37" s="3" t="n">
         <v>1</v>
@@ -1389,236 +1386,236 @@
         <v>0</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="B38" s="2" t="s">
-        <v>48</v>
-      </c>
       <c r="C38" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E38" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="C39" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E39" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B40" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="C40" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E40" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C41" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E41" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C42" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E42" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F42" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C43" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E43" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C44" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E44" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E45" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C46" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E46" s="3" t="n">
         <v>1</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>60</v>
-      </c>
       <c r="C47" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E47" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" s="3" t="n">
         <v>1</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E48" s="3" t="n">
         <v>0</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B49" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B49" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C49" s="3" t="n">
         <v>1</v>
       </c>
@@ -1629,15 +1626,15 @@
         <v>0</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C50" s="3" t="n">
         <v>2</v>
@@ -1649,15 +1646,15 @@
         <v>1</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C51" s="3" t="n">
         <v>1</v>
@@ -1669,15 +1666,15 @@
         <v>1</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C52" s="3" t="n">
         <v>1</v>
@@ -1689,15 +1686,15 @@
         <v>1</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C53" s="3" t="n">
         <v>1</v>
@@ -1709,15 +1706,15 @@
         <v>0</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C54" s="3" t="n">
         <v>1</v>
@@ -1729,15 +1726,15 @@
         <v>0</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C55" s="3" t="n">
         <v>1</v>
@@ -1749,15 +1746,15 @@
         <v>1</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C56" s="3" t="n">
         <v>1</v>
@@ -1769,15 +1766,15 @@
         <v>0</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C57" s="3" t="n">
         <v>1</v>
@@ -1789,15 +1786,15 @@
         <v>1</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C58" s="3" t="n">
         <v>1</v>
@@ -1809,15 +1806,15 @@
         <v>1</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C59" s="3" t="n">
         <v>1</v>
@@ -1829,16 +1826,16 @@
         <v>0</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B60" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="C60" s="3" t="n">
         <v>1</v>
       </c>
@@ -1849,15 +1846,15 @@
         <v>0</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C61" s="3" t="n">
         <v>1</v>
@@ -1869,15 +1866,15 @@
         <v>0</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C62" s="3" t="n">
         <v>2</v>
@@ -1889,27 +1886,27 @@
         <v>0</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B63" s="9" t="s">
-        <v>79</v>
-      </c>
       <c r="C63" s="10" t="n">
         <v>1</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E63" s="10" t="n">
         <v>0</v>
       </c>
       <c r="F63" s="12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>